<commit_message>
creating list of countries and coordinates
</commit_message>
<xml_diff>
--- a/Source/NewLocationData.xlsx
+++ b/Source/NewLocationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\Github\team-tumbleweed-data-analysis.github.io\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDED03D8-6EC3-4A4F-888A-68B8031588C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDF99FD-C66C-44CB-9B3B-50704737A54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
     <col min="2" max="2" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>